<commit_message>
created simplified stl files for openGL
</commit_message>
<xml_diff>
--- a/Private Dancer Bom.xlsx
+++ b/Private Dancer Bom.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="612">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="810" uniqueCount="613">
   <si>
     <t>#</t>
   </si>
@@ -1834,9 +1834,6 @@
     <t>Servo Arm Hitec 38mm</t>
   </si>
   <si>
-    <t>Stewart platform</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -1846,19 +1843,25 @@
     <t>stock</t>
   </si>
   <si>
-    <t>https://www.hoelleinshop.com/Sender-Servos-etc-/Servozubehoer/Servohebel-und-scheiben/fuer-Hitec/Servohebel-38mm-ohne-Versatz-Typ-A-fuer-Hitec-Servos-Carbonverstaerkt.htm?shop=hoellein&amp;SessionId=&amp;a=article&amp;ProdNr=GG992902HI&amp;t=182&amp;c=36219&amp;p=36219</t>
-  </si>
-  <si>
-    <t>https://www.hoelleinshop.com/Zubehoer/Ruderanlenkung/Kugelgelenke/Kugelgelenk-M2-mit-4-8mm-Flanschkugel-2mm-Bohrung-.htm?shop=hoellein&amp;a=article&amp;ProdNr=GG993008&amp;t=49303&amp;c=26253&amp;p=26253</t>
-  </si>
-  <si>
-    <t>12x Kugelgelenk M2</t>
-  </si>
-  <si>
-    <t>https://www.hoelleinshop.com/Zubehoer/Ruderanlenkung/Kugelgelenke/Kugelgelenk-M3-mit-4-8mm-Flanschkugel-2mm-Bohrung-.htm?shop=hoellein&amp;SessionId=&amp;a=article&amp;ProdNr=GG993010&amp;t=49303&amp;c=26253&amp;p=26253</t>
-  </si>
-  <si>
-    <t>12x Kugelgelenk M3</t>
+    <t>http://www.gabriel-stahlformenbau.de/shop/Modellbau/Kugelgelenke/Kugelgelenk-993009?source=2&amp;refertype=1&amp;referid=12</t>
+  </si>
+  <si>
+    <t>http://www.gabriel-stahlformenbau.de/shop/Modellbau/Servohebel/CFK-Servohebel-992902?source=2&amp;refertype=1&amp;referid=11</t>
+  </si>
+  <si>
+    <t>https://www.final-modellbau.de/de/zubehoer/servo-zubehoer/kugelkopf-metall-silber-15mm-m2-5-gewinde.html</t>
+  </si>
+  <si>
+    <t>12x Kugelgelenk M2.5 CFK</t>
+  </si>
+  <si>
+    <t>12x Kugelgelenk M2.5 Metall</t>
+  </si>
+  <si>
+    <t>Stewart platform rods</t>
+  </si>
+  <si>
+    <t>Stewart platform  Servo</t>
   </si>
 </sst>
 </file>
@@ -5381,7 +5384,7 @@
   <dimension ref="B2:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -5423,7 +5426,7 @@
         <v>6</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>604</v>
+        <v>603</v>
       </c>
     </row>
     <row r="3" spans="2:11" x14ac:dyDescent="0.35">
@@ -5450,7 +5453,7 @@
         <v>59</v>
       </c>
       <c r="K3" s="394" t="s">
-        <v>605</v>
+        <v>604</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.35">
@@ -5477,7 +5480,7 @@
         <v>29.95</v>
       </c>
       <c r="K4" s="394" t="s">
-        <v>606</v>
+        <v>605</v>
       </c>
     </row>
     <row r="5" spans="2:11" x14ac:dyDescent="0.35">
@@ -5488,7 +5491,7 @@
         <v>602</v>
       </c>
       <c r="D5" s="394" t="s">
-        <v>603</v>
+        <v>612</v>
       </c>
       <c r="G5" s="391" t="s">
         <v>607</v>
@@ -5500,7 +5503,7 @@
         <v>3.9</v>
       </c>
       <c r="J5" s="392">
-        <f t="shared" ref="J5:J7" si="1">I5*B5</f>
+        <f t="shared" ref="J5:J6" si="1">I5*B5</f>
         <v>23.4</v>
       </c>
       <c r="K5" s="394"/>
@@ -5513,44 +5516,44 @@
         <v>609</v>
       </c>
       <c r="D6" s="394" t="s">
-        <v>603</v>
+        <v>611</v>
       </c>
       <c r="G6" s="391" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="H6" s="394">
         <v>10</v>
       </c>
       <c r="I6" s="593">
-        <v>9.9</v>
+        <v>10.9</v>
       </c>
       <c r="J6" s="392">
-        <f t="shared" si="1"/>
-        <v>19.8</v>
+        <f>I6*B6</f>
+        <v>21.8</v>
       </c>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="394">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="C7" s="394" t="s">
+        <v>610</v>
+      </c>
+      <c r="D7" s="394" t="s">
         <v>611</v>
       </c>
-      <c r="D7" s="394" t="s">
-        <v>603</v>
-      </c>
       <c r="G7" s="391" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
       <c r="H7" s="394">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="I7" s="593">
-        <v>11.35</v>
+        <v>1.95</v>
       </c>
       <c r="J7" s="392">
-        <f t="shared" si="1"/>
-        <v>22.7</v>
+        <f>I7*B7</f>
+        <v>23.4</v>
       </c>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.35">

</xml_diff>